<commit_message>
Fehlermeldung für fehlerhafte Tabellen.
</commit_message>
<xml_diff>
--- a/static/file/uploads/Projekt.xlsx
+++ b/static/file/uploads/Projekt.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -80,16 +80,19 @@
     <t xml:space="preserve">E,F</t>
   </si>
   <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schnarchen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vorname</t>
   </si>
   <si>
     <t xml:space="preserve">Nachname</t>
   </si>
   <si>
-    <t xml:space="preserve">Arbeitspackete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
+    <t xml:space="preserve">Arbeitspakete</t>
   </si>
   <si>
     <t xml:space="preserve">SM</t>
@@ -101,10 +104,7 @@
     <t xml:space="preserve">Mann</t>
   </si>
   <si>
-    <t xml:space="preserve">A,B:50,C:25,D,F,G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">super@mann.de</t>
+    <t xml:space="preserve">A,B,C:75,E:25,D:25,F:75,G,H</t>
   </si>
   <si>
     <t xml:space="preserve">PL</t>
@@ -116,10 +116,7 @@
     <t xml:space="preserve">Langstrumpf</t>
   </si>
   <si>
-    <t xml:space="preserve">A,B:50,C:75,E,G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pippi@villa-kunterbunt.sl</t>
+    <t xml:space="preserve">A,B,C:25,E:75,D:75,F:25,G:50,H</t>
   </si>
 </sst>
 </file>
@@ -194,9 +191,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -216,128 +217,424 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="6" style="1" width="3.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="50" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
+      <c r="T1" s="0"/>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
+      <c r="AH1" s="0"/>
+      <c r="AI1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
+      <c r="AF3" s="0"/>
+      <c r="AG3" s="0"/>
+      <c r="AH3" s="0"/>
+      <c r="AI3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
+      <c r="AG5" s="0"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0"/>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
+      <c r="T6" s="0"/>
+      <c r="U6" s="0"/>
+      <c r="V6" s="0"/>
+      <c r="W6" s="0"/>
+      <c r="X6" s="0"/>
+      <c r="Y6" s="0"/>
+      <c r="Z6" s="0"/>
+      <c r="AA6" s="0"/>
+      <c r="AB6" s="0"/>
+      <c r="AC6" s="0"/>
+      <c r="AD6" s="0"/>
+      <c r="AE6" s="0"/>
+      <c r="AF6" s="0"/>
+      <c r="AG6" s="0"/>
+      <c r="AH6" s="0"/>
+      <c r="AI6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
+      <c r="AE7" s="0"/>
+      <c r="AF7" s="0"/>
+      <c r="AG7" s="0"/>
+      <c r="AH7" s="0"/>
+      <c r="AI7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0"/>
+      <c r="AE8" s="0"/>
+      <c r="AF8" s="0"/>
+      <c r="AG8" s="0"/>
+      <c r="AH8" s="0"/>
+      <c r="AI8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="Z9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="0"/>
+      <c r="AC9" s="0"/>
+      <c r="AD9" s="0"/>
+      <c r="AE9" s="0"/>
+      <c r="AF9" s="0"/>
+      <c r="AG9" s="0"/>
+      <c r="AH9" s="0"/>
+      <c r="AI9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -355,18 +652,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,32 +669,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>27</v>
       </c>
     </row>
@@ -415,9 +704,6 @@
       </c>
       <c r="D3" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>